<commit_message>
Modification to CSV processor, Finish Map layout
</commit_message>
<xml_diff>
--- a/Dantong Xue_Sprint0/Game1/Game1/Code/LoadFile/test_colored.xlsx
+++ b/Dantong Xue_Sprint0/Game1/Game1/Code/LoadFile/test_colored.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repo\CSE-3902\Dantong Xue_Sprint0\Game1\Game1\Code\LoadFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{80CABBD9-CEA6-4A08-93B3-D501CA2873CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB3BE5C-37D3-4959-92BD-CECC7C80DA46}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="6">
   <si>
     <t>lockedDoorFront</t>
     <phoneticPr fontId="19" type="noConversion"/>
@@ -41,11 +41,14 @@
     <t>block</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
+  <si>
+    <t>_</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1059,11 +1062,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1072,40 +1075,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
+      <c r="A1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="O1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
+      <c r="P1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
@@ -1126,38 +1191,102 @@
       <c r="AX1" s="1"/>
     </row>
     <row r="2" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
-      <c r="Y2" s="4"/>
-      <c r="Z2" s="4"/>
-      <c r="AA2" s="4"/>
-      <c r="AB2" s="4"/>
-      <c r="AC2" s="2"/>
-      <c r="AD2" s="2"/>
-      <c r="AE2" s="2"/>
-      <c r="AF2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF2" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="AG2" s="1"/>
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
@@ -1178,38 +1307,102 @@
       <c r="AX2" s="1"/>
     </row>
     <row r="3" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="2"/>
-      <c r="AD3" s="2"/>
-      <c r="AE3" s="2"/>
-      <c r="AF3" s="2"/>
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="AG3" s="1"/>
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
@@ -1230,38 +1423,102 @@
       <c r="AX3" s="1"/>
     </row>
     <row r="4" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-      <c r="Z4" s="4"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="2"/>
-      <c r="AE4" s="2"/>
-      <c r="AF4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF4" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="AG4" s="1"/>
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
@@ -1282,10 +1539,18 @@
       <c r="AX4" s="1"/>
     </row>
     <row r="5" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1334,10 +1599,18 @@
         <v>4</v>
       </c>
       <c r="AB5" s="6"/>
-      <c r="AC5" s="4"/>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="4"/>
-      <c r="AF5" s="4"/>
+      <c r="AC5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
@@ -1358,10 +1631,18 @@
       <c r="AX5" s="1"/>
     </row>
     <row r="6" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -1386,10 +1667,18 @@
       <c r="Z6" s="6"/>
       <c r="AA6" s="6"/>
       <c r="AB6" s="6"/>
-      <c r="AC6" s="4"/>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="4"/>
-      <c r="AF6" s="4"/>
+      <c r="AC6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF6" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG6" s="1"/>
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
@@ -1410,10 +1699,18 @@
       <c r="AX6" s="1"/>
     </row>
     <row r="7" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>4</v>
       </c>
@@ -1462,10 +1759,18 @@
         <v>4</v>
       </c>
       <c r="AB7" s="6"/>
-      <c r="AC7" s="4"/>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="4"/>
-      <c r="AF7" s="4"/>
+      <c r="AC7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF7" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG7" s="1"/>
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
@@ -1486,10 +1791,18 @@
       <c r="AX7" s="1"/>
     </row>
     <row r="8" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
@@ -1514,10 +1827,18 @@
       <c r="Z8" s="6"/>
       <c r="AA8" s="6"/>
       <c r="AB8" s="6"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
+      <c r="AC8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF8" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG8" s="1"/>
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
@@ -1538,10 +1859,18 @@
       <c r="AX8" s="1"/>
     </row>
     <row r="9" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E9" s="6" t="s">
         <v>4</v>
       </c>
@@ -1590,10 +1919,18 @@
         <v>4</v>
       </c>
       <c r="AB9" s="6"/>
-      <c r="AC9" s="4"/>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="4"/>
-      <c r="AF9" s="4"/>
+      <c r="AC9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG9" s="1"/>
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
@@ -1617,9 +1954,15 @@
       <c r="A10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -1647,9 +1990,15 @@
       <c r="AC10" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AD10" s="5"/>
-      <c r="AE10" s="5"/>
-      <c r="AF10" s="5"/>
+      <c r="AD10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AG10" s="1"/>
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
@@ -1670,10 +2019,18 @@
       <c r="AX10" s="1"/>
     </row>
     <row r="11" spans="1:50" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E11" s="6" t="s">
         <v>4</v>
       </c>
@@ -1722,10 +2079,18 @@
         <v>4</v>
       </c>
       <c r="AB11" s="6"/>
-      <c r="AC11" s="5"/>
-      <c r="AD11" s="5"/>
-      <c r="AE11" s="5"/>
-      <c r="AF11" s="5"/>
+      <c r="AC11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AG11" s="1"/>
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
@@ -1746,10 +2111,18 @@
       <c r="AX11" s="1"/>
     </row>
     <row r="12" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
@@ -1774,10 +2147,18 @@
       <c r="Z12" s="6"/>
       <c r="AA12" s="6"/>
       <c r="AB12" s="6"/>
-      <c r="AC12" s="5"/>
-      <c r="AD12" s="5"/>
-      <c r="AE12" s="5"/>
-      <c r="AF12" s="5"/>
+      <c r="AC12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF12" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
@@ -1798,10 +2179,18 @@
       <c r="AX12" s="1"/>
     </row>
     <row r="13" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="A13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="E13" s="6" t="s">
         <v>4</v>
       </c>
@@ -1850,10 +2239,18 @@
         <v>4</v>
       </c>
       <c r="AB13" s="6"/>
-      <c r="AC13" s="5"/>
-      <c r="AD13" s="5"/>
-      <c r="AE13" s="5"/>
-      <c r="AF13" s="5"/>
+      <c r="AC13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF13" s="5" t="s">
+        <v>5</v>
+      </c>
       <c r="AG13" s="1"/>
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
@@ -1874,10 +2271,18 @@
       <c r="AX13" s="1"/>
     </row>
     <row r="14" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
@@ -1902,10 +2307,18 @@
       <c r="Z14" s="6"/>
       <c r="AA14" s="6"/>
       <c r="AB14" s="6"/>
-      <c r="AC14" s="4"/>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4"/>
+      <c r="AC14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG14" s="1"/>
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
@@ -1926,10 +2339,18 @@
       <c r="AX14" s="1"/>
     </row>
     <row r="15" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E15" s="6" t="s">
         <v>4</v>
       </c>
@@ -1978,10 +2399,18 @@
         <v>4</v>
       </c>
       <c r="AB15" s="6"/>
-      <c r="AC15" s="4"/>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="4"/>
-      <c r="AF15" s="4"/>
+      <c r="AC15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF15" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG15" s="1"/>
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
@@ -2002,10 +2431,18 @@
       <c r="AX15" s="1"/>
     </row>
     <row r="16" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
@@ -2030,10 +2467,18 @@
       <c r="Z16" s="6"/>
       <c r="AA16" s="6"/>
       <c r="AB16" s="6"/>
-      <c r="AC16" s="4"/>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="4"/>
-      <c r="AF16" s="4"/>
+      <c r="AC16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF16" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
@@ -2054,10 +2499,18 @@
       <c r="AX16" s="1"/>
     </row>
     <row r="17" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E17" s="6" t="s">
         <v>4</v>
       </c>
@@ -2106,10 +2559,18 @@
         <v>4</v>
       </c>
       <c r="AB17" s="6"/>
-      <c r="AC17" s="4"/>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="4"/>
-      <c r="AF17" s="4"/>
+      <c r="AC17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG17" s="1"/>
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
@@ -2130,10 +2591,18 @@
       <c r="AX17" s="1"/>
     </row>
     <row r="18" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
@@ -2158,10 +2627,18 @@
       <c r="Z18" s="6"/>
       <c r="AA18" s="6"/>
       <c r="AB18" s="6"/>
-      <c r="AC18" s="4"/>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="4"/>
-      <c r="AF18" s="4"/>
+      <c r="AC18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF18" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="AG18" s="1"/>
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
@@ -2182,40 +2659,102 @@
       <c r="AX18" s="1"/>
     </row>
     <row r="19" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N19" s="4" t="s">
+        <v>5</v>
+      </c>
       <c r="O19" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="5"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="4"/>
-      <c r="V19" s="4"/>
-      <c r="W19" s="4"/>
-      <c r="X19" s="4"/>
-      <c r="Y19" s="4"/>
-      <c r="Z19" s="4"/>
-      <c r="AA19" s="4"/>
-      <c r="AB19" s="4"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
+      <c r="P19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF19" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="AG19" s="1"/>
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
@@ -2236,38 +2775,102 @@
       <c r="AX19" s="1"/>
     </row>
     <row r="20" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="5"/>
-      <c r="P20" s="5"/>
-      <c r="Q20" s="5"/>
-      <c r="R20" s="5"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
-      <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF20" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="AG20" s="1"/>
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
@@ -2288,38 +2891,102 @@
       <c r="AX20" s="1"/>
     </row>
     <row r="21" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="5"/>
-      <c r="P21" s="5"/>
-      <c r="Q21" s="5"/>
-      <c r="R21" s="5"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="3"/>
-      <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
-      <c r="AF21" s="3"/>
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF21" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="AG21" s="1"/>
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
@@ -2340,38 +3007,102 @@
       <c r="AX21" s="1"/>
     </row>
     <row r="22" spans="1:50" ht="14.4" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-      <c r="M22" s="4"/>
-      <c r="N22" s="4"/>
-      <c r="O22" s="5"/>
-      <c r="P22" s="5"/>
-      <c r="Q22" s="5"/>
-      <c r="R22" s="5"/>
-      <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4"/>
-      <c r="V22" s="4"/>
-      <c r="W22" s="4"/>
-      <c r="X22" s="4"/>
-      <c r="Y22" s="4"/>
-      <c r="Z22" s="4"/>
-      <c r="AA22" s="4"/>
-      <c r="AB22" s="4"/>
-      <c r="AC22" s="3"/>
-      <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
-      <c r="AF22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="O22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="P22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="R22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="T22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="U22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="W22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="X22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AB22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AD22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AE22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AF22" s="3" t="s">
+        <v>5</v>
+      </c>
       <c r="AG22" s="1"/>
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
@@ -2809,11 +3540,78 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="Q17:R18"/>
-    <mergeCell ref="S17:T18"/>
-    <mergeCell ref="U17:V18"/>
-    <mergeCell ref="W17:X18"/>
-    <mergeCell ref="Y17:Z18"/>
+    <mergeCell ref="AA5:AB6"/>
+    <mergeCell ref="E5:F6"/>
+    <mergeCell ref="G5:H6"/>
+    <mergeCell ref="I5:J6"/>
+    <mergeCell ref="K5:L6"/>
+    <mergeCell ref="M5:N6"/>
+    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="Q5:R6"/>
+    <mergeCell ref="S5:T6"/>
+    <mergeCell ref="U5:V6"/>
+    <mergeCell ref="W5:X6"/>
+    <mergeCell ref="Y5:Z6"/>
+    <mergeCell ref="AA7:AB8"/>
+    <mergeCell ref="E7:F8"/>
+    <mergeCell ref="G7:H8"/>
+    <mergeCell ref="I7:J8"/>
+    <mergeCell ref="K7:L8"/>
+    <mergeCell ref="M7:N8"/>
+    <mergeCell ref="O7:P8"/>
+    <mergeCell ref="Q7:R8"/>
+    <mergeCell ref="S7:T8"/>
+    <mergeCell ref="U7:V8"/>
+    <mergeCell ref="W7:X8"/>
+    <mergeCell ref="Y7:Z8"/>
+    <mergeCell ref="AA9:AB10"/>
+    <mergeCell ref="E9:F10"/>
+    <mergeCell ref="G9:H10"/>
+    <mergeCell ref="I9:J10"/>
+    <mergeCell ref="K9:L10"/>
+    <mergeCell ref="M9:N10"/>
+    <mergeCell ref="O9:P10"/>
+    <mergeCell ref="Q9:R10"/>
+    <mergeCell ref="S9:T10"/>
+    <mergeCell ref="U9:V10"/>
+    <mergeCell ref="W9:X10"/>
+    <mergeCell ref="Y9:Z10"/>
+    <mergeCell ref="AA11:AB12"/>
+    <mergeCell ref="E11:F12"/>
+    <mergeCell ref="G11:H12"/>
+    <mergeCell ref="I11:J12"/>
+    <mergeCell ref="K11:L12"/>
+    <mergeCell ref="M11:N12"/>
+    <mergeCell ref="O11:P12"/>
+    <mergeCell ref="Q11:R12"/>
+    <mergeCell ref="S11:T12"/>
+    <mergeCell ref="U11:V12"/>
+    <mergeCell ref="W11:X12"/>
+    <mergeCell ref="Y11:Z12"/>
+    <mergeCell ref="AA13:AB14"/>
+    <mergeCell ref="E13:F14"/>
+    <mergeCell ref="G13:H14"/>
+    <mergeCell ref="I13:J14"/>
+    <mergeCell ref="K13:L14"/>
+    <mergeCell ref="M13:N14"/>
+    <mergeCell ref="O13:P14"/>
+    <mergeCell ref="Q13:R14"/>
+    <mergeCell ref="S13:T14"/>
+    <mergeCell ref="U13:V14"/>
+    <mergeCell ref="W13:X14"/>
+    <mergeCell ref="Y13:Z14"/>
+    <mergeCell ref="AA15:AB16"/>
+    <mergeCell ref="E15:F16"/>
+    <mergeCell ref="G15:H16"/>
+    <mergeCell ref="I15:J16"/>
+    <mergeCell ref="K15:L16"/>
+    <mergeCell ref="M15:N16"/>
+    <mergeCell ref="O15:P16"/>
+    <mergeCell ref="Q15:R16"/>
+    <mergeCell ref="S15:T16"/>
+    <mergeCell ref="U15:V16"/>
+    <mergeCell ref="W15:X16"/>
+    <mergeCell ref="Y15:Z16"/>
     <mergeCell ref="AA17:AB18"/>
     <mergeCell ref="E17:F18"/>
     <mergeCell ref="G17:H18"/>
@@ -2821,78 +3619,11 @@
     <mergeCell ref="K17:L18"/>
     <mergeCell ref="M17:N18"/>
     <mergeCell ref="O17:P18"/>
-    <mergeCell ref="Q15:R16"/>
-    <mergeCell ref="S15:T16"/>
-    <mergeCell ref="U15:V16"/>
-    <mergeCell ref="W15:X16"/>
-    <mergeCell ref="Y15:Z16"/>
-    <mergeCell ref="AA15:AB16"/>
-    <mergeCell ref="E15:F16"/>
-    <mergeCell ref="G15:H16"/>
-    <mergeCell ref="I15:J16"/>
-    <mergeCell ref="K15:L16"/>
-    <mergeCell ref="M15:N16"/>
-    <mergeCell ref="O15:P16"/>
-    <mergeCell ref="Q13:R14"/>
-    <mergeCell ref="S13:T14"/>
-    <mergeCell ref="U13:V14"/>
-    <mergeCell ref="W13:X14"/>
-    <mergeCell ref="Y13:Z14"/>
-    <mergeCell ref="AA13:AB14"/>
-    <mergeCell ref="E13:F14"/>
-    <mergeCell ref="G13:H14"/>
-    <mergeCell ref="I13:J14"/>
-    <mergeCell ref="K13:L14"/>
-    <mergeCell ref="M13:N14"/>
-    <mergeCell ref="O13:P14"/>
-    <mergeCell ref="Q11:R12"/>
-    <mergeCell ref="S11:T12"/>
-    <mergeCell ref="U11:V12"/>
-    <mergeCell ref="W11:X12"/>
-    <mergeCell ref="Y11:Z12"/>
-    <mergeCell ref="AA11:AB12"/>
-    <mergeCell ref="E11:F12"/>
-    <mergeCell ref="G11:H12"/>
-    <mergeCell ref="I11:J12"/>
-    <mergeCell ref="K11:L12"/>
-    <mergeCell ref="M11:N12"/>
-    <mergeCell ref="O11:P12"/>
-    <mergeCell ref="Q9:R10"/>
-    <mergeCell ref="S9:T10"/>
-    <mergeCell ref="U9:V10"/>
-    <mergeCell ref="W9:X10"/>
-    <mergeCell ref="Y9:Z10"/>
-    <mergeCell ref="AA9:AB10"/>
-    <mergeCell ref="E9:F10"/>
-    <mergeCell ref="G9:H10"/>
-    <mergeCell ref="I9:J10"/>
-    <mergeCell ref="K9:L10"/>
-    <mergeCell ref="M9:N10"/>
-    <mergeCell ref="O9:P10"/>
-    <mergeCell ref="Q7:R8"/>
-    <mergeCell ref="S7:T8"/>
-    <mergeCell ref="U7:V8"/>
-    <mergeCell ref="W7:X8"/>
-    <mergeCell ref="Y7:Z8"/>
-    <mergeCell ref="AA7:AB8"/>
-    <mergeCell ref="E7:F8"/>
-    <mergeCell ref="G7:H8"/>
-    <mergeCell ref="I7:J8"/>
-    <mergeCell ref="K7:L8"/>
-    <mergeCell ref="M7:N8"/>
-    <mergeCell ref="O7:P8"/>
-    <mergeCell ref="Q5:R6"/>
-    <mergeCell ref="S5:T6"/>
-    <mergeCell ref="U5:V6"/>
-    <mergeCell ref="W5:X6"/>
-    <mergeCell ref="Y5:Z6"/>
-    <mergeCell ref="AA5:AB6"/>
-    <mergeCell ref="E5:F6"/>
-    <mergeCell ref="G5:H6"/>
-    <mergeCell ref="I5:J6"/>
-    <mergeCell ref="K5:L6"/>
-    <mergeCell ref="M5:N6"/>
-    <mergeCell ref="O5:P6"/>
+    <mergeCell ref="Q17:R18"/>
+    <mergeCell ref="S17:T18"/>
+    <mergeCell ref="U17:V18"/>
+    <mergeCell ref="W17:X18"/>
+    <mergeCell ref="Y17:Z18"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>